<commit_message>
Final touches, go live
</commit_message>
<xml_diff>
--- a/uploads/contacts_template.xlsx
+++ b/uploads/contacts_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ncda\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC553CE1-ED4B-4506-A39D-DD2C63D15077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97FC08D6-7332-49E9-818D-A660116D2DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{26F30B74-6D89-4656-ACC4-EC0B9C0DE296}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{26F30B74-6D89-4656-ACC4-EC0B9C0DE296}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>FIRSTNAME</t>
   </si>
@@ -59,6 +57,9 @@
   </si>
   <si>
     <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>DESIGNATION</t>
   </si>
 </sst>
 </file>
@@ -419,21 +420,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5AE3CA-1042-4B73-83CB-F0C8FB937052}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="6" max="6" width="18.36328125" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,6 +459,9 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>